<commit_message>
adding a website address
</commit_message>
<xml_diff>
--- a/Przypakdki testowe,Karolina Sandak.xlsx
+++ b/Przypakdki testowe,Karolina Sandak.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertsandak/Documents/Karolinka/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertsandak/Documents/Karolinka/Przypadki testowe/Test-Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73632676-458C-574F-A222-A7C5896B8D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022E3F68-210D-5245-8707-5365098BBF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" xr2:uid="{657EE937-9D79-D94D-899C-D575821EDB6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Nazwa</t>
   </si>
@@ -110,12 +110,15 @@
   <si>
     <t>Rejestracja nowego klienta</t>
   </si>
+  <si>
+    <t>Przypadki testowe do sklepu internetowego https://magento2-demo.magebit.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,8 +146,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -181,17 +197,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE59ABB-EF6A-3343-82B5-839668F6C64B}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,108 +583,100 @@
     <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="325" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:6" ht="250" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>